<commit_message>
Changes to cohorts content
</commit_message>
<xml_diff>
--- a/app/files/historic-vaccination-records-import-template.xlsx
+++ b/app/files/historic-vaccination-records-import-template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28723"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4085F1EB-7F50-4BF6-A65E-C2DA4F4820DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB35E6F1-6FAC-43C6-A1E0-550FDF427592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,7 +147,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
       </rPr>
-      <t>. Must be formatted as a valid postcode</t>
+      <t>. Must be one of Not known, Male, Female, Not specified.</t>
     </r>
   </si>
   <si>
@@ -166,7 +166,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
       </rPr>
-      <t>. Must use either YYYMMDD or DD/M/YYYY formats</t>
+      <t>. Must be a valid UK postcode</t>
     </r>
   </si>
   <si>
@@ -216,7 +216,7 @@
     <t>Optional. Must be 6 digits and numeric. Use 888888 for school unknown and 999999 for homeschooled.</t>
   </si>
   <si>
-    <t>Required if SCHOOL_URN is 888888</t>
+    <t>Required only if SCHOOL_URN is 888888</t>
   </si>
   <si>
     <t>Optional. Must be 10 digits and numeric</t>
@@ -234,13 +234,13 @@
     <t>Optional. Must use either YYYYMMDD or DD/MM/YYYY</t>
   </si>
   <si>
-    <t>Required if VACCINE_GIVEN is omitted. Must be Y or N</t>
+    <t>Required only if VACCINE_GIVEN is omitted. Must be Y or N</t>
   </si>
   <si>
     <t>Optional. It must be appropriate for the vaccine delivery method and be one of: left arm (lower position), left arm (upper position), left buttock, left thigh, left upper arm, nasal, right arm (lower position), right arm (upper position), right buttock, right thigh or right upper arm</t>
   </si>
   <si>
-    <t>Required if VACCINATED is N, must be absent from school, already had elsewhere, did not attend, refused, unwell or vaccination contraindicated</t>
+    <t>Required only if VACCINATED is N. Must be absent from school, already had elsewhere, did not attend, refused, unwell or vaccination contraindicated</t>
   </si>
   <si>
     <t>Optional. Must be a number or 1B, 1P, 2B, 2P or 3P</t>
@@ -249,7 +249,7 @@
     <t>Optional. Must be 1 (school) or 2 (clinic)</t>
   </si>
   <si>
-    <t>Required if CARE_SETTING is 2, must be the name of a community clinic location</t>
+    <t>Required only if CARE_SETTING is 2. Must be the name of a community clinic location</t>
   </si>
 </sst>
 </file>
@@ -326,13 +326,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,11 +675,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="77" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="51.5703125" customWidth="1"/>
+    <col min="17" max="17" width="228.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="123.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="69" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="38" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" t="s">
@@ -752,7 +783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" ht="29.25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -762,7 +793,7 @@
       <c r="C2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -798,13 +829,13 @@
       <c r="O2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="Q2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="6" t="s">
         <v>41</v>
       </c>
       <c r="S2" t="s">
@@ -816,7 +847,7 @@
       <c r="U2" t="s">
         <v>43</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="W2" t="s">

</xml_diff>